<commit_message>
update Cơ sở dữ liệu đồ án 2.xlsx
</commit_message>
<xml_diff>
--- a/Document/Cơ sở dữ liệu đồ án 2.xlsx
+++ b/Document/Cơ sở dữ liệu đồ án 2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>careers</t>
   </si>
@@ -85,34 +85,40 @@
     <t>register_time</t>
   </si>
   <si>
+    <t>status (hoàn thành|chưa đủ số lượng|đang tiến trình|...)</t>
+  </si>
+  <si>
+    <t>teacher_id</t>
+  </si>
+  <si>
     <t>schedule</t>
   </si>
   <si>
-    <t>status (hoàn thành|chưa đủ số lượng|đang tiến trình|...)</t>
-  </si>
-  <si>
-    <t>teacher_id</t>
-  </si>
-  <si>
     <t>subject_id</t>
   </si>
   <si>
+    <t>period</t>
+  </si>
+  <si>
     <t>attendances</t>
   </si>
   <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>is_hoc_bu</t>
+  </si>
+  <si>
     <t>attendance_class</t>
   </si>
   <si>
     <t>attendance_id</t>
   </si>
   <si>
-    <t>period</t>
-  </si>
-  <si>
-    <t>status (vắng|đến trễ|có phép|...)</t>
-  </si>
-  <si>
-    <t>time</t>
+    <t>is_present</t>
   </si>
 </sst>
 </file>
@@ -147,7 +153,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +170,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -203,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -221,6 +239,12 @@
     </xf>
     <xf borderId="3" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,60 +629,80 @@
       <c r="A22" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="s">
-        <v>26</v>
+      <c r="A23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="s">
-        <v>27</v>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C27" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="C28" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="s">
+      <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="s">
-        <v>19</v>
+      <c r="A32" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="s">
-        <v>32</v>
+      <c r="A34" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>